<commit_message>
Made 4_plots_or.qmd for odds ratio
</commit_message>
<xml_diff>
--- a/Data/ODE data v3.xlsx
+++ b/Data/ODE data v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073A1978-09A6-4943-B5AC-B1DC8D2418A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4DEE46-3B8C-4E47-B4D8-10DF27777E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1020" yWindow="1900" windowWidth="21820" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11380" yWindow="11000" windowWidth="21820" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3919,7 +3919,10 @@
       <c r="R78" s="20"/>
     </row>
     <row r="79" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C79" s="1"/>
+      <c r="C79" s="1">
+        <f>SUM(C2:C78)</f>
+        <v>36089</v>
+      </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>

</xml_diff>

<commit_message>
Made dq_native and dq_hispanic  (df/csv) in 4_plots_or.qmd  - odds ratio
</commit_message>
<xml_diff>
--- a/Data/ODE data v3.xlsx
+++ b/Data/ODE data v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4DEE46-3B8C-4E47-B4D8-10DF27777E23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94495524-4CCA-C147-9F17-AD0753561DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11380" yWindow="11000" windowWidth="21820" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3920" yWindow="500" windowWidth="22100" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -686,8 +686,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R978"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -935,7 +936,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="6">
-        <f>SUM(D7:L7)</f>
+        <f t="shared" ref="C7:C12" si="0">SUM(D7:L7)</f>
         <v>2</v>
       </c>
       <c r="D7" s="6">
@@ -974,7 +975,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="6">
-        <f>SUM(D8:L8)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D8" s="10">
@@ -1013,7 +1014,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="6">
-        <f>SUM(D9:L9)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D9" s="12">
@@ -1052,7 +1053,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="6">
-        <f>SUM(D10:L10)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D10" s="6">
@@ -1091,7 +1092,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="6">
-        <f>SUM(D11:L11)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D11" s="6">
@@ -1130,7 +1131,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="6">
-        <f>SUM(D12:L12)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D12" s="6">
@@ -1359,7 +1360,7 @@
         <v>11</v>
       </c>
       <c r="C18" s="6">
-        <f>SUM(D18:L18)</f>
+        <f t="shared" ref="C18:C23" si="1">SUM(D18:L18)</f>
         <v>2900</v>
       </c>
       <c r="D18" s="12">
@@ -1398,7 +1399,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="6">
-        <f>SUM(D19:L19)</f>
+        <f t="shared" si="1"/>
         <v>3007</v>
       </c>
       <c r="D19" s="6">
@@ -1437,7 +1438,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="6">
-        <f>SUM(D20:L20)</f>
+        <f t="shared" si="1"/>
         <v>2418</v>
       </c>
       <c r="D20" s="6">
@@ -1476,7 +1477,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="6">
-        <f>SUM(D21:L21)</f>
+        <f t="shared" si="1"/>
         <v>2520</v>
       </c>
       <c r="D21" s="10">
@@ -1515,7 +1516,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="6">
-        <f>SUM(D22:L22)</f>
+        <f t="shared" si="1"/>
         <v>2680</v>
       </c>
       <c r="D22" s="12">
@@ -1554,7 +1555,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="6">
-        <f>SUM(D23:L23)</f>
+        <f t="shared" si="1"/>
         <v>3003</v>
       </c>
       <c r="D23" s="6">
@@ -1783,7 +1784,7 @@
         <v>11</v>
       </c>
       <c r="C29" s="6">
-        <f>SUM(D29:L29)</f>
+        <f t="shared" ref="C29:C34" si="2">SUM(D29:L29)</f>
         <v>426</v>
       </c>
       <c r="D29" s="6">
@@ -1822,7 +1823,7 @@
         <v>19</v>
       </c>
       <c r="C30" s="6">
-        <f>SUM(D30:L30)</f>
+        <f t="shared" si="2"/>
         <v>475</v>
       </c>
       <c r="D30" s="10">
@@ -1861,7 +1862,7 @@
         <v>19</v>
       </c>
       <c r="C31" s="6">
-        <f>SUM(D31:L31)</f>
+        <f t="shared" si="2"/>
         <v>342</v>
       </c>
       <c r="D31" s="12">
@@ -1900,7 +1901,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="6">
-        <f>SUM(D32:L32)</f>
+        <f t="shared" si="2"/>
         <v>458</v>
       </c>
       <c r="D32" s="6">
@@ -1939,7 +1940,7 @@
         <v>21</v>
       </c>
       <c r="C33" s="6">
-        <f>SUM(D33:L33)</f>
+        <f t="shared" si="2"/>
         <v>520</v>
       </c>
       <c r="D33" s="6">
@@ -1978,7 +1979,7 @@
         <v>22</v>
       </c>
       <c r="C34" s="6">
-        <f>SUM(D34:L34)</f>
+        <f t="shared" si="2"/>
         <v>504</v>
       </c>
       <c r="D34" s="6">
@@ -2207,7 +2208,7 @@
         <v>11</v>
       </c>
       <c r="C40" s="6">
-        <f>SUM(D40:L40)</f>
+        <f t="shared" ref="C40:C45" si="3">SUM(D40:L40)</f>
         <v>9</v>
       </c>
       <c r="D40" s="6">
@@ -2246,7 +2247,7 @@
         <v>19</v>
       </c>
       <c r="C41" s="6">
-        <f>SUM(D41:L41)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="D41" s="6">
@@ -2288,7 +2289,7 @@
         <v>20</v>
       </c>
       <c r="C42" s="6">
-        <f>SUM(D42:L42)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="D42" s="10">
@@ -2327,7 +2328,7 @@
         <v>21</v>
       </c>
       <c r="C43" s="6">
-        <f>SUM(D43:L43)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="D43" s="12">
@@ -2366,7 +2367,7 @@
         <v>21</v>
       </c>
       <c r="C44" s="41">
-        <f>SUM(D44:L44)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="D44" s="41">
@@ -2411,7 +2412,7 @@
         <v>22</v>
       </c>
       <c r="C45" s="42">
-        <f>SUM(D45:L45)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="D45" s="42">
@@ -2676,7 +2677,7 @@
         <v>11</v>
       </c>
       <c r="C51" s="41">
-        <f>SUM(D51:L51)</f>
+        <f t="shared" ref="C51:C56" si="4">SUM(D51:L51)</f>
         <v>0</v>
       </c>
       <c r="D51" s="41">
@@ -2721,7 +2722,7 @@
         <v>19</v>
       </c>
       <c r="C52" s="42">
-        <f>SUM(D52:L52)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D52" s="42">
@@ -2766,7 +2767,7 @@
         <v>20</v>
       </c>
       <c r="C53" s="42">
-        <f>SUM(D53:L53)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D53" s="42">
@@ -2811,7 +2812,7 @@
         <v>21</v>
       </c>
       <c r="C54" s="42">
-        <f>SUM(D54:L54)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D54" s="42">
@@ -2856,7 +2857,7 @@
         <v>21</v>
       </c>
       <c r="C55" s="42">
-        <f>SUM(D55:L55)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="D55" s="42">
@@ -2901,7 +2902,7 @@
         <v>22</v>
       </c>
       <c r="C56" s="42">
-        <f>SUM(D56:L56)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="D56" s="42">
@@ -3166,7 +3167,7 @@
         <v>11</v>
       </c>
       <c r="C62" s="42">
-        <f>SUM(D62:L62)</f>
+        <f t="shared" ref="C62:C67" si="5">SUM(D62:L62)</f>
         <v>414</v>
       </c>
       <c r="D62" s="42">
@@ -3211,7 +3212,7 @@
         <v>19</v>
       </c>
       <c r="C63" s="42">
-        <f>SUM(D63:L63)</f>
+        <f t="shared" si="5"/>
         <v>353</v>
       </c>
       <c r="D63" s="42">
@@ -3256,7 +3257,7 @@
         <v>20</v>
       </c>
       <c r="C64" s="43">
-        <f>SUM(D64:L64)</f>
+        <f t="shared" si="5"/>
         <v>305</v>
       </c>
       <c r="D64" s="43">
@@ -3301,7 +3302,7 @@
         <v>21</v>
       </c>
       <c r="C65" s="41">
-        <f>SUM(D65:L65)</f>
+        <f t="shared" si="5"/>
         <v>330</v>
       </c>
       <c r="D65" s="41">
@@ -3346,7 +3347,7 @@
         <v>21</v>
       </c>
       <c r="C66" s="42">
-        <f>SUM(D66:L66)</f>
+        <f t="shared" si="5"/>
         <v>338</v>
       </c>
       <c r="D66" s="42">
@@ -3391,7 +3392,7 @@
         <v>22</v>
       </c>
       <c r="C67" s="42">
-        <f>SUM(D67:L67)</f>
+        <f t="shared" si="5"/>
         <v>328</v>
       </c>
       <c r="D67" s="42">
@@ -3656,7 +3657,7 @@
         <v>11</v>
       </c>
       <c r="C73" s="42">
-        <f>SUM(D73:L73)</f>
+        <f t="shared" ref="C73:C78" si="6">SUM(D73:L73)</f>
         <v>8</v>
       </c>
       <c r="D73" s="42">
@@ -3701,7 +3702,7 @@
         <v>19</v>
       </c>
       <c r="C74" s="42">
-        <f>SUM(D74:L74)</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="D74" s="42">
@@ -3746,7 +3747,7 @@
         <v>20</v>
       </c>
       <c r="C75" s="42">
-        <f>SUM(D75:L75)</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="D75" s="42">
@@ -3791,7 +3792,7 @@
         <v>21</v>
       </c>
       <c r="C76" s="42">
-        <f>SUM(D76:L76)</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="D76" s="42">
@@ -3836,7 +3837,7 @@
         <v>21</v>
       </c>
       <c r="C77" s="42">
-        <f>SUM(D77:L77)</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="D77" s="42">
@@ -3881,7 +3882,7 @@
         <v>22</v>
       </c>
       <c r="C78" s="43">
-        <f>SUM(D78:L78)</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="D78" s="43">
@@ -3919,10 +3920,7 @@
       <c r="R78" s="20"/>
     </row>
     <row r="79" spans="1:18" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C79" s="1">
-        <f>SUM(C2:C78)</f>
-        <v>36089</v>
-      </c>
+      <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>

</xml_diff>

<commit_message>
1b_child_counts_and_census.qmd - udpated numbers for CC, census, updated chi-sq, corrplots circle/number for racial representations (NATIONAL)
</commit_message>
<xml_diff>
--- a/Data/ODE data v3.xlsx
+++ b/Data/ODE data v3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Desktop/EDLD652_Diss/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94495524-4CCA-C147-9F17-AD0753561DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1875449-599E-8F42-96B6-6907832A90C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="500" windowWidth="22100" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1820" windowWidth="23040" windowHeight="15760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -687,8 +687,8 @@
   <dimension ref="A1:R978"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E83" sqref="E83"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>